<commit_message>
updated busted DK PN
</commit_message>
<xml_diff>
--- a/TPS40305_supply BOM.xlsx
+++ b/TPS40305_supply BOM.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skot/Work/Bitcoin/TPS40305_supply/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{098F0D35-CAC2-624B-9017-EB73163FCDAD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0608155F-B6D4-9F4F-80D2-2D9B737F3B62}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11580" yWindow="5400" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="11580" yWindow="5400" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TPS40305_supply" sheetId="1" r:id="rId1"/>
+    <sheet name="DK Order" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="78">
   <si>
     <t>Qty</t>
   </si>
@@ -214,9 +215,6 @@
     <t>10k</t>
   </si>
   <si>
-    <t>13-RC0402JR-1310KLTR-ND</t>
-  </si>
-  <si>
     <t>R6</t>
   </si>
   <si>
@@ -254,12 +252,15 @@
   </si>
   <si>
     <t>J1, J2, J3, J4</t>
+  </si>
+  <si>
+    <t>311-10KJRCT-ND</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1094,11 +1095,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1131,7 +1132,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -1280,7 +1281,7 @@
         <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C12" t="s">
         <v>37</v>
@@ -1410,7 +1411,7 @@
         <v>63</v>
       </c>
       <c r="D20" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -1418,47 +1419,319 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21" t="s">
         <v>65</v>
+      </c>
+      <c r="D21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" t="s">
+        <v>69</v>
+      </c>
+      <c r="E22" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" t="s">
+        <v>72</v>
+      </c>
+      <c r="D23" t="s">
+        <v>73</v>
+      </c>
+      <c r="E23" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{668F4A0D-F7D0-6247-8E37-9D8358EDFB4D}">
+  <dimension ref="A1:C23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="12.83203125" customWidth="1"/>
+    <col min="3" max="3" width="26.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>64</v>
       </c>
       <c r="C21" t="s">
         <v>66</v>
       </c>
-      <c r="D21" t="s">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
         <v>67</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>1</v>
-      </c>
-      <c r="B22" t="s">
-        <v>68</v>
       </c>
       <c r="C22" t="s">
         <v>69</v>
       </c>
-      <c r="D22" t="s">
-        <v>70</v>
-      </c>
-      <c r="E22" t="s">
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>1</v>
-      </c>
-      <c r="B23" t="s">
-        <v>72</v>
       </c>
       <c r="C23" t="s">
         <v>73</v>
-      </c>
-      <c r="D23" t="s">
-        <v>74</v>
-      </c>
-      <c r="E23" t="s">
-        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>